<commit_message>
Updated IEPD adding codes and SID.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="157">
   <si>
     <t>Data Item</t>
   </si>
@@ -431,28 +431,7 @@
     <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonSexText</t>
-  </si>
-  <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonRaceText</t>
-  </si>
-  <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonHeightMeasure/nc:MeasureValueText</t>
-  </si>
-  <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonWeightMeasure/nc:MeasureValueText</t>
-  </si>
-  <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonEyeColorText</t>
-  </si>
-  <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonHairColorText</t>
-  </si>
-  <si>
     <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonResidenceAssociation/nc:Location/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:AddressFullText</t>
   </si>
   <si>
     <t>/cdr-report-doc:CourtDispositionRecordingReport/cdr-report-ext:CycleTrackingIdentification/nc:IdentificationID</t>
@@ -585,6 +564,44 @@
   <si>
     <t>Notes:
 Remove Chargesubject from NIEM</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>State Identification Number</t>
+  </si>
+  <si>
+    <t>/cdr-report-doc:CourtDispositionRecordingReport/nc:Person[@s:id/cdr-report-doc:CourtDispositionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/cdr-report-doc:CourtDispositionRecordingReport/nc:Person/nc:PersonStateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonResidenceAssociation/nc:Location/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:LocationStreet/nc:StreetFullText
+/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonResidenceAssociation/nc:Location/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:LocationCityName
+/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonResidenceAssociation/nc:Location/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc-3.0.1:LocationStateUSPostalServiceCode
+/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonResidenceAssociation/nc:Location/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:LocationPostalExtensionCode</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/j:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonHeightMeasure/nc:MeasureValueText
+/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonHeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonWeightMeasure/nc:MeasureValueText
+/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/j:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/j:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonStateIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -783,6 +800,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -794,18 +823,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1108,56 +1125,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D40" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="126.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="166.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="126.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="166.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="180" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="159.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15" t="s">
+      <c r="A1" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="16" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1173,13 +1190,13 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>96</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1196,13 +1213,13 @@
         <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>97</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1217,7 +1234,7 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1235,7 +1252,7 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1252,7 +1269,7 @@
         <v>98</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1266,7 +1283,7 @@
         <v>32</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F8" s="8"/>
     </row>
@@ -1281,7 +1298,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -1300,7 +1317,7 @@
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1318,7 +1335,7 @@
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1336,7 +1353,7 @@
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1354,7 +1371,7 @@
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="5" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1382,7 +1399,7 @@
         <v>71</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>99</v>
@@ -1390,7 +1407,7 @@
     </row>
     <row r="16" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>73</v>
@@ -1413,7 +1430,7 @@
         <v>78</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F17" s="8"/>
     </row>
@@ -1428,7 +1445,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F18" s="8"/>
     </row>
@@ -1441,7 +1458,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F19" s="8"/>
     </row>
@@ -1451,7 +1468,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="E20" s="7" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F20" s="8"/>
     </row>
@@ -1466,7 +1483,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -1479,7 +1496,7 @@
         <v>33</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -1491,7 +1508,7 @@
         <v>90</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F23" s="8"/>
     </row>
@@ -1501,7 +1518,7 @@
       </c>
       <c r="B24" s="4"/>
       <c r="E24" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F24" s="8"/>
     </row>
@@ -1514,7 +1531,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F25" s="8"/>
     </row>
@@ -1527,7 +1544,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -1542,13 +1559,13 @@
         <v>11</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -1565,13 +1582,13 @@
         <v>35</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1579,7 +1596,7 @@
         <v>61</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>102</v>
@@ -1587,197 +1604,211 @@
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>62</v>
+        <v>146</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="F32" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D35" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="D38" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="E39" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="17" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="11"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Incorporated the "Disposition Reporting Service" disposition codes into the SSP.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="154">
   <si>
     <t>Data Item</t>
   </si>
@@ -402,9 +402,6 @@
     <t>Probation Conditions</t>
   </si>
   <si>
-    <t>Full Text Address?</t>
-  </si>
-  <si>
     <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/pdr-report-ext:CycleTrackingIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -475,12 +472,6 @@
     <t>/cdr-report-doc:CourtDispositionRecordingReport/nc:Disposition/nc:DispositionEntity/nc:EntityOrganization[@s:id/cdr-report-doc:CourtDispositionRecordingReport/nc:Disposition/nc:DispositionEntity/nc:EntityOrganization/@s:ref]/cdr-report-doc:CourtDispositionRecordingReport/nc:Organization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/nc:ActivityCategoryText</t>
-  </si>
-  <si>
-    <t>/cdr-report-doc:CourtDispositionRecordingReport/nc:Disposition/nc:DispositionCategoryText</t>
-  </si>
-  <si>
     <t>/cdr-report-doc:CourtDispositionRecordingReport/nc:Disposition/nc:DispositionDate/nc:Date</t>
   </si>
   <si>
@@ -551,12 +542,6 @@
   </si>
   <si>
     <t>DECLINE</t>
-  </si>
-  <si>
-    <t>Text or Codes?</t>
-  </si>
-  <si>
-    <t>Do we need an element for unit of measure?</t>
   </si>
   <si>
     <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceGroupingText</t>
@@ -602,6 +587,12 @@
   </si>
   <si>
     <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonStateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cdr-report-doc:CourtDispositionRecordingReport/nc:Disposition/me_disposition_codes:CourtActionCode</t>
+  </si>
+  <si>
+    <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/me_disposition_codes:SentenceTermCategoryCode</t>
   </si>
 </sst>
 </file>
@@ -1127,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1135,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1190,13 +1181,13 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1213,13 +1204,13 @@
         <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1234,7 +1225,7 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1252,7 +1243,7 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1266,10 +1257,10 @@
         <v>32</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1283,7 +1274,7 @@
         <v>32</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F8" s="8"/>
     </row>
@@ -1298,7 +1289,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -1317,7 +1308,7 @@
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1335,7 +1326,7 @@
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1353,7 +1344,7 @@
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1371,7 +1362,7 @@
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="5" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1399,15 +1390,15 @@
         <v>71</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>73</v>
@@ -1419,7 +1410,7 @@
         <v>74</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1430,7 +1421,7 @@
         <v>78</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F17" s="8"/>
     </row>
@@ -1445,7 +1436,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="F18" s="8"/>
     </row>
@@ -1458,7 +1449,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F19" s="8"/>
     </row>
@@ -1468,7 +1459,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="E20" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F20" s="8"/>
     </row>
@@ -1483,7 +1474,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -1496,7 +1487,7 @@
         <v>33</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -1508,7 +1499,7 @@
         <v>90</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F23" s="8"/>
     </row>
@@ -1518,7 +1509,7 @@
       </c>
       <c r="B24" s="4"/>
       <c r="E24" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F24" s="8"/>
     </row>
@@ -1531,7 +1522,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F25" s="8"/>
     </row>
@@ -1544,7 +1535,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -1559,13 +1550,13 @@
         <v>11</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -1582,13 +1573,13 @@
         <v>35</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1596,24 +1587,24 @@
         <v>61</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1621,84 +1612,63 @@
         <v>62</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="5" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="F32" s="8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="F33" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="F34" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="F35" s="8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="F36" s="8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="F37" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="F38" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1715,13 +1685,13 @@
         <v>53</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1739,7 +1709,7 @@
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1757,10 +1727,10 @@
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>49</v>
       </c>
@@ -1775,7 +1745,7 @@
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1793,7 +1763,7 @@
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.25">
@@ -1801,7 +1771,7 @@
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="4"/>

</xml_diff>

<commit_message>
Moved the ChargeToCourtIndicator and EndProsecutorChargeCycleIndicator properties to “Charge” in the Prosecution-Decision-Recording Report.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
@@ -411,12 +411,6 @@
     <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:CaseProsecutionAttorney/pdr-report-ext:ProsecutionAttorneyOrganization/@s:ref]/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/pdr-report-ext:ChargeToCourtIndicator</t>
-  </si>
-  <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/pdr-report-ext:EndProsecutorChargeCycleIndicator</t>
-  </si>
-  <si>
     <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonGivenName
 /pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonMiddleName
 /pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonSurName</t>
@@ -593,6 +587,12 @@
   </si>
   <si>
     <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/me_disposition_codes:SentenceTermCategoryCode</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/pdr-report-ext:ChargeToCourtIndicator</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/pdr-report-ext:EndProsecutorChargeCycleIndicator</t>
   </si>
 </sst>
 </file>
@@ -1118,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="F8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1135,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1181,13 +1181,13 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>95</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1204,13 +1204,13 @@
         <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>96</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1260,7 +1260,7 @@
         <v>97</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,7 +1274,7 @@
         <v>32</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F8" s="8"/>
     </row>
@@ -1289,7 +1289,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="5" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1390,15 +1390,15 @@
         <v>71</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>73</v>
@@ -1410,7 +1410,7 @@
         <v>74</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
         <v>78</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F17" s="8"/>
     </row>
@@ -1436,7 +1436,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F18" s="8"/>
     </row>
@@ -1449,7 +1449,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F19" s="8"/>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="E20" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F20" s="8"/>
     </row>
@@ -1474,7 +1474,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -1487,7 +1487,7 @@
         <v>33</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -1499,7 +1499,7 @@
         <v>90</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F23" s="8"/>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B24" s="4"/>
       <c r="E24" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F24" s="8"/>
     </row>
@@ -1522,7 +1522,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F25" s="8"/>
     </row>
@@ -1535,7 +1535,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -1550,13 +1550,13 @@
         <v>11</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -1573,13 +1573,13 @@
         <v>35</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1587,24 +1587,24 @@
         <v>61</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="F30" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
         <v>62</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="5" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1620,7 +1620,7 @@
         <v>63</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1628,7 +1628,7 @@
         <v>64</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
         <v>65</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1644,7 +1644,7 @@
         <v>66</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1652,7 +1652,7 @@
         <v>67</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>68</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
         <v>69</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1685,13 +1685,13 @@
         <v>53</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1727,7 +1727,7 @@
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.25">
@@ -1771,7 +1771,7 @@
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="4"/>

</xml_diff>

<commit_message>
Merged master to analytical data store branch.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
@@ -411,12 +411,6 @@
     <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:CaseProsecutionAttorney/pdr-report-ext:ProsecutionAttorneyOrganization/@s:ref]/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/pdr-report-ext:ChargeToCourtIndicator</t>
-  </si>
-  <si>
-    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/pdr-report-ext:EndProsecutorChargeCycleIndicator</t>
-  </si>
-  <si>
     <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonGivenName
 /pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonMiddleName
 /pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person[@s:id/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Subject/nc:RoleOfPerson/@s:ref]/pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonSurName</t>
@@ -593,6 +587,12 @@
   </si>
   <si>
     <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/me_disposition_codes:SentenceTermCategoryCode</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/pdr-report-ext:ChargeToCourtIndicator</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/pdr-report-ext:EndProsecutorChargeCycleIndicator</t>
   </si>
 </sst>
 </file>
@@ -1118,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="F8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1135,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1181,13 +1181,13 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>95</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1204,13 +1204,13 @@
         <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>96</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1260,7 +1260,7 @@
         <v>97</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,7 +1274,7 @@
         <v>32</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F8" s="8"/>
     </row>
@@ -1289,7 +1289,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="5" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1390,15 +1390,15 @@
         <v>71</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>73</v>
@@ -1410,7 +1410,7 @@
         <v>74</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
         <v>78</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F17" s="8"/>
     </row>
@@ -1436,7 +1436,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F18" s="8"/>
     </row>
@@ -1449,7 +1449,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F19" s="8"/>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="E20" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F20" s="8"/>
     </row>
@@ -1474,7 +1474,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -1487,7 +1487,7 @@
         <v>33</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -1499,7 +1499,7 @@
         <v>90</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F23" s="8"/>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B24" s="4"/>
       <c r="E24" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F24" s="8"/>
     </row>
@@ -1522,7 +1522,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F25" s="8"/>
     </row>
@@ -1535,7 +1535,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -1550,13 +1550,13 @@
         <v>11</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -1573,13 +1573,13 @@
         <v>35</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1587,24 +1587,24 @@
         <v>61</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="F30" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
         <v>62</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="5" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1620,7 +1620,7 @@
         <v>63</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1628,7 +1628,7 @@
         <v>64</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
         <v>65</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1644,7 +1644,7 @@
         <v>66</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1652,7 +1652,7 @@
         <v>67</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>68</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
         <v>69</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1685,13 +1685,13 @@
         <v>53</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1727,7 +1727,7 @@
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.25">
@@ -1771,7 +1771,7 @@
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="4"/>

</xml_diff>

<commit_message>
Made the following changes to the Court-Disposition-Recording-Report in the Criminal_History_Update_Reporting_Service:
SENTENCE
1.	Update to include both  “FeeAmount” and “RestitutionAmount” 
2.	Added “TermDurationRemaining” as a property of
“SentenceSuspendedTerm”
3.	Added TermLifeIndicator
ASSOCIATIONS
Added:
1.	PersonChargeAssociation
2.	ActivityChargeAssociation  -  Where “Activity “ is “Sentence”
3.	ChargeDispositionAssociation
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Update_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Update_Report-IEPD/documentation/Criminal_History_Update_Mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="161">
   <si>
     <t>Data Item</t>
   </si>
@@ -384,9 +384,6 @@
     <t>E.g., incarcerated, fined, etc.</t>
   </si>
   <si>
-    <t>Sentence Amount</t>
-  </si>
-  <si>
     <t>E.g., Length of time, amount of fine, etc.</t>
   </si>
   <si>
@@ -455,11 +452,6 @@
     <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceCondition/nc:ActivityDescriptionText</t>
   </si>
   <si>
-    <t xml:space="preserve">/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceCondition/nc:ConditionDisciplinaryAction/nc:DisciplinaryActionFee/nc:ObligationDueAmount/nc:Amount
-/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceTerm/j:TermDuration
-</t>
-  </si>
-  <si>
     <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceIssuerEntity/nc:EntityOrganization[@s:id/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceIssuerEntity/nc:EntityOrganization/@s:ref]/cdr-report-doc:CourtDispositionRecordingReport/nc:Organization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -593,6 +585,33 @@
   </si>
   <si>
     <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/pdr-report-ext:EndProsecutorChargeCycleIndicator</t>
+  </si>
+  <si>
+    <t>Sentence Fee</t>
+  </si>
+  <si>
+    <t>Sentence Term</t>
+  </si>
+  <si>
+    <t>Sentence Restitution</t>
+  </si>
+  <si>
+    <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceCondition/nc:ConditionDisciplinaryAction/nc:DisciplinaryActionFee/nc:ObligationDueAmount/nc:Amount</t>
+  </si>
+  <si>
+    <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceCondition/nc:ConditionDisciplinaryAction/nc:DisciplinaryActionRestitution/nc:ObligationDueAmount/nc:Amount</t>
+  </si>
+  <si>
+    <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceTerm/j:TermDuration</t>
+  </si>
+  <si>
+    <t>Suspended Sentence Term Remaining</t>
+  </si>
+  <si>
+    <t>Life Sentence Indicator</t>
+  </si>
+  <si>
+    <t>/cdr-report-doc:CourtDispositionRecordingReport/j:Sentence/j:SentenceTerm/j:TermLifeIndicator</t>
   </si>
 </sst>
 </file>
@@ -1116,16 +1135,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="126.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="166.85546875" style="3" customWidth="1"/>
@@ -1135,7 +1154,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1181,13 +1200,13 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1204,13 +1223,13 @@
         <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1225,7 +1244,7 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1243,7 +1262,7 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1257,10 +1276,10 @@
         <v>32</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,7 +1293,7 @@
         <v>32</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F8" s="8"/>
     </row>
@@ -1289,7 +1308,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -1308,7 +1327,7 @@
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1326,7 +1345,7 @@
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1344,7 +1363,7 @@
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1362,7 +1381,7 @@
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="5" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1390,15 +1409,15 @@
         <v>71</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>73</v>
@@ -1410,7 +1429,7 @@
         <v>74</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1421,7 +1440,7 @@
         <v>78</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F17" s="8"/>
     </row>
@@ -1436,7 +1455,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F18" s="8"/>
     </row>
@@ -1449,7 +1468,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F19" s="8"/>
     </row>
@@ -1459,7 +1478,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="E20" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F20" s="8"/>
     </row>
@@ -1474,311 +1493,347 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="7" t="s">
         <v>33</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:7" s="7" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="E23" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" s="7" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" s="7" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" s="7" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" s="7" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="E24" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="B28" s="4"/>
+      <c r="E28" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="7" t="s">
+      <c r="B30" s="4"/>
+      <c r="C30" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="7" t="s">
+      <c r="E30" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" s="5" customFormat="1" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="8" t="s">
+      <c r="E31" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F32" s="8" t="s">
-        <v>142</v>
+        <v>103</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>65</v>
+        <v>137</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>139</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="5" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="5" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F38" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="F42" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D43" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G39" s="5" t="s">
+      <c r="E43" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="5" t="s">
+    <row r="46" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="5" t="s">
+    <row r="47" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="11"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+    <row r="48" spans="1:7" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48" s="11"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>